<commit_message>
body map conda added in tomer
</commit_message>
<xml_diff>
--- a/Debug Output/debug_trials_dichotic_session_DICHOTIC_PRE.xlsx
+++ b/Debug Output/debug_trials_dichotic_session_DICHOTIC_PRE.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -54,18 +54,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -391,12 +391,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sentence ntr - 87</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 59</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -409,12 +409,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 105</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sentence neg - 120</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -427,12 +427,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sentence ntr - 91</t>
+          <t>Sentence ntr - 87</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 7</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -445,12 +445,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sentence ntr - 91</t>
+          <t>Sentence ntr - 98</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 134</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -463,12 +463,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sentence ntr - 76</t>
+          <t>Sentence ntr - 69</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sentence neg - 131</t>
+          <t>Sentence neg - 123</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -481,12 +481,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Sentence ntr - 98</t>
+          <t>Sentence ntr - 69</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Sentence neg - 22</t>
+          <t>Sentence neg - 123</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -499,12 +499,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sentence ntr - 98</t>
+          <t>Sentence ntr - 114</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sentence neg - 35</t>
+          <t>Sentence neg - 48</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -517,12 +517,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Sentence ntr - 109</t>
+          <t>Sentence ntr - 96</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Sentence neg - 128</t>
+          <t>Sentence neg - 126</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -535,7 +535,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Sentence ntr - 115</t>
+          <t>Sentence ntr - 96</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -553,7 +553,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Sentence ntr - 96</t>
+          <t>Sentence ntr - 97</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -571,12 +571,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Sentence ntr - 119</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Sentence neg - 66</t>
+          <t>Sentence neg - 129</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -589,12 +589,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Sentence neg - 9</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -607,12 +607,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Sentence ntr - 109</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Sentence neg - 22</t>
+          <t>Sentence neg - 10</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -625,12 +625,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Sentence ntr - 96</t>
+          <t>Sentence ntr - 114</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Sentence neg - 26</t>
+          <t>Sentence neg - 123</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -643,12 +643,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Sentence neg - 10</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -661,12 +661,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 105</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Sentence neg - 10</t>
+          <t>Sentence neg - 129</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -679,12 +679,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Sentence ntr - 119</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Sentence neg - 120</t>
+          <t>Sentence neg - 59</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -697,12 +697,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 69</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -715,12 +715,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Sentence ntr - 114</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Sentence neg - 35</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -733,12 +733,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Sentence ntr - 91</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -751,7 +751,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Sentence ntr - 91</t>
+          <t>Sentence ntr - 87</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -774,7 +774,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Sentence neg - 25</t>
+          <t>Sentence neg - 48</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -787,12 +787,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Sentence ntr - 70</t>
+          <t>Sentence ntr - 98</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 48</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -805,12 +805,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Sentence ntr - 103</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Sentence neg - 131</t>
+          <t>Sentence neg - 126</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -823,12 +823,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 105</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Sentence neg - 120</t>
+          <t>Sentence neg - 134</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -841,12 +841,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Sentence ntr - 119</t>
+          <t>Sentence ntr - 87</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Sentence neg - 66</t>
+          <t>Sentence neg - 129</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -859,12 +859,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Sentence ntr - 87</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Sentence neg - 128</t>
+          <t>Sentence neg - 123</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -877,12 +877,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Sentence ntr - 87</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Sentence neg - 128</t>
+          <t>Sentence neg - 123</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -895,12 +895,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Sentence ntr - 109</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Sentence neg - 9</t>
+          <t>Sentence neg - 59</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -913,12 +913,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Sentence ntr - 109</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Sentence neg - 22</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -931,12 +931,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Sentence ntr - 70</t>
+          <t>Sentence ntr - 97</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 7</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -949,12 +949,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Sentence ntr - 96</t>
+          <t>Sentence ntr - 97</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Sentence neg - 25</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -967,12 +967,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 114</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Sentence neg - 26</t>
+          <t>Sentence neg - 10</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -985,12 +985,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Sentence ntr - 98</t>
+          <t>Sentence ntr - 114</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Sentence neg - 131</t>
+          <t>Sentence neg - 10</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1003,12 +1003,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Sentence ntr - 114</t>
+          <t>Sentence ntr - 69</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Sentence neg - 131</t>
+          <t>Sentence neg - 126</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1021,12 +1021,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Sentence ntr - 115</t>
+          <t>Sentence ntr - 93</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1039,12 +1039,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 69</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Sentence neg - 120</t>
+          <t>Sentence neg - 10</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1057,12 +1057,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Sentence ntr - 70</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 134</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1075,12 +1075,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Sentence ntr - 96</t>
+          <t>Sentence ntr - 98</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Sentence neg - 66</t>
+          <t>Sentence neg - 48</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1093,12 +1093,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Sentence ntr - 96</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Sentence neg - 66</t>
+          <t>Sentence neg - 48</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1111,12 +1111,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Sentence ntr - 115</t>
+          <t>Sentence ntr - 93</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 7</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1129,12 +1129,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Sentence ntr - 103</t>
+          <t>Sentence ntr - 93</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Sentence neg - 35</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1147,12 +1147,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 114</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Sentence neg - 10</t>
+          <t>Sentence neg - 59</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1165,12 +1165,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Sentence ntr - 76</t>
+          <t>Sentence ntr - 114</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 129</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1183,12 +1183,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Sentence ntr - 119</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Sentence neg - 9</t>
+          <t>Sentence neg - 126</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1201,12 +1201,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Sentence ntr - 109</t>
+          <t>Sentence ntr - 96</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Sentence neg - 22</t>
+          <t>Sentence neg - 126</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1219,12 +1219,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Sentence ntr - 109</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Sentence neg - 22</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1237,12 +1237,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Sentence ntr - 87</t>
+          <t>Sentence ntr - 97</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Sentence neg - 26</t>
+          <t>Sentence neg - 123</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1255,12 +1255,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 69</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Sentence neg - 26</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1273,12 +1273,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Sentence ntr - 114</t>
+          <t>Sentence ntr - 98</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 129</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1291,12 +1291,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Sentence ntr - 76</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Sentence neg - 35</t>
+          <t>Sentence neg - 126</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1309,12 +1309,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Sentence ntr - 76</t>
+          <t>Sentence ntr - 114</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Sentence neg - 35</t>
+          <t>Sentence neg - 123</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1327,12 +1327,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Sentence ntr - 70</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Sentence neg - 25</t>
+          <t>Sentence neg - 134</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1345,12 +1345,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Sentence ntr - 87</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Sentence neg - 120</t>
+          <t>Sentence neg - 134</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1363,12 +1363,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Sentence ntr - 109</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Sentence neg - 9</t>
+          <t>Sentence neg - 10</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1381,12 +1381,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Sentence ntr - 98</t>
+          <t>Sentence ntr - 96</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Sentence neg - 131</t>
+          <t>Sentence neg - 59</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1399,12 +1399,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Sentence ntr - 98</t>
+          <t>Sentence ntr - 96</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Sentence neg - 131</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1417,12 +1417,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Sentence ntr - 96</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Sentence neg - 128</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1435,12 +1435,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Sentence ntr - 103</t>
+          <t>Sentence ntr - 97</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Sentence neg - 22</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1453,12 +1453,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 105</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Sentence neg - 10</t>
+          <t>Sentence neg - 48</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1471,12 +1471,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Sentence ntr - 114</t>
+          <t>Sentence ntr - 69</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Sentence neg - 10</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1489,12 +1489,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Sentence ntr - 103</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Sentence neg - 120</t>
+          <t>Sentence neg - 134</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1507,12 +1507,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Sentence ntr - 76</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Sentence neg - 25</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1525,12 +1525,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Sentence ntr - 70</t>
+          <t>Sentence ntr - 114</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Sentence neg - 26</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1543,12 +1543,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Sentence ntr - 98</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Sentence neg - 22</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1561,12 +1561,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Sentence ntr - 98</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Sentence neg - 22</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1579,12 +1579,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Sentence neg - 66</t>
+          <t>Sentence neg - 7</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1597,12 +1597,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Sentence ntr - 91</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Sentence neg - 66</t>
+          <t>Sentence neg - 7</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1633,12 +1633,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Sentence ntr - 96</t>
+          <t>Sentence ntr - 93</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Sentence neg - 131</t>
+          <t>Sentence neg - 123</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -1651,12 +1651,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 126</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -1669,12 +1669,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Sentence ntr - 87</t>
+          <t>Sentence ntr - 105</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Sentence neg - 128</t>
+          <t>Sentence neg - 48</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -1687,12 +1687,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Sentence ntr - 87</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Sentence neg - 26</t>
+          <t>Sentence neg - 129</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -1705,12 +1705,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Sentence ntr - 96</t>
+          <t>Sentence ntr - 87</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Sentence neg - 35</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -1723,12 +1723,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Sentence ntr - 98</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Sentence neg - 66</t>
+          <t>Sentence neg - 126</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -1741,12 +1741,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Sentence ntr - 98</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Sentence neg - 66</t>
+          <t>Sentence neg - 10</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -1759,12 +1759,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Sentence ntr - 109</t>
+          <t>Sentence ntr - 69</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -1777,12 +1777,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Sentence ntr - 119</t>
+          <t>Sentence ntr - 69</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Sentence neg - 131</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -1795,12 +1795,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Sentence ntr - 114</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 134</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -1813,12 +1813,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Sentence ntr - 114</t>
+          <t>Sentence ntr - 96</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 134</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -1831,12 +1831,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Sentence ntr - 115</t>
+          <t>Sentence ntr - 97</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1849,12 +1849,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 105</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Sentence neg - 120</t>
+          <t>Sentence neg - 48</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -1867,12 +1867,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Sentence ntr - 76</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Sentence neg - 10</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -1885,12 +1885,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Sentence ntr - 91</t>
+          <t>Sentence ntr - 93</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Sentence neg - 9</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -1903,12 +1903,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Sentence neg - 9</t>
+          <t>Sentence neg - 59</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -1921,12 +1921,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Sentence ntr - 115</t>
+          <t>Sentence ntr - 96</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Sentence neg - 66</t>
+          <t>Sentence neg - 10</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -1939,12 +1939,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Sentence ntr - 109</t>
+          <t>Sentence ntr - 98</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Sentence neg - 128</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -1957,12 +1957,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Sentence ntr - 109</t>
+          <t>Sentence ntr - 98</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Sentence neg - 35</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -1975,12 +1975,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Sentence ntr - 103</t>
+          <t>Sentence ntr - 105</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -1993,12 +1993,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Sentence ntr - 103</t>
+          <t>Sentence ntr - 87</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -2011,12 +2011,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Sentence ntr - 70</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Sentence neg - 120</t>
+          <t>Sentence neg - 126</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -2029,12 +2029,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Sentence ntr - 76</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Sentence neg - 26</t>
+          <t>Sentence neg - 129</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -2047,12 +2047,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Sentence ntr - 114</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 129</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -2065,12 +2065,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Sentence ntr - 91</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -2083,12 +2083,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Sentence ntr - 87</t>
+          <t>Sentence ntr - 97</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -2101,12 +2101,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Sentence ntr - 98</t>
+          <t>Sentence ntr - 114</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Sentence neg - 10</t>
+          <t>Sentence neg - 7</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -2119,12 +2119,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Sentence ntr - 109</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Sentence neg - 22</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -2137,12 +2137,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Sentence ntr - 76</t>
+          <t>Sentence ntr - 69</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Sentence neg - 128</t>
+          <t>Sentence neg - 48</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -2155,12 +2155,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Sentence ntr - 115</t>
+          <t>Sentence ntr - 97</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Sentence neg - 131</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -2173,12 +2173,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Sentence ntr - 119</t>
+          <t>Sentence ntr - 97</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -2191,12 +2191,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Sentence ntr - 91</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Sentence neg - 9</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -2209,12 +2209,12 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Sentence ntr - 91</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Sentence neg - 25</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -2227,12 +2227,12 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 98</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Sentence neg - 120</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -2245,12 +2245,12 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Sentence ntr - 87</t>
+          <t>Sentence ntr - 93</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Sentence neg - 120</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -2263,12 +2263,12 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Sentence ntr - 96</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 59</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -2281,12 +2281,12 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Sentence ntr - 70</t>
+          <t>Sentence ntr - 105</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 134</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -2299,12 +2299,12 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Sentence ntr - 70</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Sentence neg - 35</t>
+          <t>Sentence neg - 129</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -2317,7 +2317,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 87</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -2335,12 +2335,12 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Sentence ntr - 91</t>
+          <t>Sentence ntr - 98</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Sentence neg - 10</t>
+          <t>Sentence neg - 7</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -2358,7 +2358,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -2371,12 +2371,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Sentence ntr - 119</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 129</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -2389,12 +2389,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Sentence ntr - 119</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 129</t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -2407,12 +2407,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Sentence ntr - 103</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Sentence neg - 26</t>
+          <t>Sentence neg - 126</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -2425,12 +2425,12 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Sentence ntr - 70</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 134</t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -2443,12 +2443,12 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Sentence ntr - 76</t>
+          <t>Sentence ntr - 105</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 123</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -2461,12 +2461,12 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Sentence ntr - 114</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Sentence neg - 22</t>
+          <t>Sentence neg - 123</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -2479,12 +2479,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Sentence ntr - 109</t>
+          <t>Sentence ntr - 97</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Sentence neg - 9</t>
+          <t>Sentence neg - 48</t>
         </is>
       </c>
       <c r="C118" t="n">
@@ -2497,12 +2497,12 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 114</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Sentence neg - 35</t>
+          <t>Sentence neg - 10</t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -2515,12 +2515,12 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 114</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Sentence neg - 120</t>
+          <t>Sentence neg - 59</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -2533,12 +2533,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 93</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Sentence neg - 128</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -2551,12 +2551,12 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Sentence ntr - 109</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Sentence neg - 131</t>
+          <t>Sentence neg - 129</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -2569,12 +2569,12 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Sentence ntr - 70</t>
+          <t>Sentence ntr - 105</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 126</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2592,7 +2592,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Sentence neg - 26</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -2610,7 +2610,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Sentence neg - 22</t>
+          <t>Sentence neg - 10</t>
         </is>
       </c>
       <c r="C125" t="n">
@@ -2623,12 +2623,12 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Sentence ntr - 114</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Sentence neg - 9</t>
+          <t>Sentence neg - 123</t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -2641,12 +2641,12 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Sentence ntr - 114</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Sentence neg - 9</t>
+          <t>Sentence neg - 123</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -2659,12 +2659,12 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Sentence ntr - 98</t>
+          <t>Sentence ntr - 69</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Sentence neg - 10</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -2677,12 +2677,12 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Sentence ntr - 103</t>
+          <t>Sentence ntr - 114</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Sentence neg - 66</t>
+          <t>Sentence neg - 7</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -2695,12 +2695,12 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Sentence ntr - 96</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Sentence neg - 66</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -2713,12 +2713,12 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Sentence neg - 35</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C131" t="n">
@@ -2731,12 +2731,12 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C132" t="n">
@@ -2749,12 +2749,12 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Sentence ntr - 119</t>
+          <t>Sentence ntr - 97</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Sentence neg - 25</t>
+          <t>Sentence neg - 134</t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -2767,12 +2767,12 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Sentence ntr - 115</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C134" t="n">
@@ -2785,12 +2785,12 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Sentence ntr - 98</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Sentence neg - 22</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C135" t="n">
@@ -2803,12 +2803,12 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Sentence ntr - 91</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Sentence neg - 9</t>
+          <t>Sentence neg - 10</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -2821,12 +2821,12 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Sentence ntr - 103</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Sentence neg - 9</t>
+          <t>Sentence neg - 129</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -2839,12 +2839,12 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Sentence ntr - 70</t>
+          <t>Sentence ntr - 93</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 7</t>
         </is>
       </c>
       <c r="C138" t="n">
@@ -2857,12 +2857,12 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Sentence ntr - 70</t>
+          <t>Sentence ntr - 93</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Sentence neg - 10</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -2875,12 +2875,12 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Sentence ntr - 114</t>
+          <t>Sentence ntr - 87</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Sentence neg - 10</t>
+          <t>Sentence neg - 59</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -2893,12 +2893,12 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Sentence ntr - 76</t>
+          <t>Sentence ntr - 114</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Sentence neg - 128</t>
+          <t>Sentence neg - 59</t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -2911,12 +2911,12 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Sentence ntr - 119</t>
+          <t>Sentence ntr - 97</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Sentence neg - 131</t>
+          <t>Sentence neg - 123</t>
         </is>
       </c>
       <c r="C142" t="n">
@@ -2929,12 +2929,12 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Sentence ntr - 119</t>
+          <t>Sentence ntr - 98</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Sentence neg - 35</t>
+          <t>Sentence neg - 123</t>
         </is>
       </c>
       <c r="C143" t="n">
@@ -2947,12 +2947,12 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Sentence neg - 26</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C144" t="n">
@@ -2965,12 +2965,12 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Sentence ntr - 109</t>
+          <t>Sentence ntr - 105</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -2981,6 +2981,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Isuues in afact and dct catch trials
</commit_message>
<xml_diff>
--- a/Debug Output/debug_trials_dichotic_session_DICHOTIC_PRE.xlsx
+++ b/Debug Output/debug_trials_dichotic_session_DICHOTIC_PRE.xlsx
@@ -391,12 +391,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sentence ntr - 113</t>
+          <t>Sentence ntr - 70</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -409,12 +409,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sentence ntr - 102</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sentence neg - 133</t>
+          <t>Sentence neg - 2</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -427,12 +427,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sentence ntr - 118</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Sentence neg - 139</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -445,12 +445,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sentence ntr - 118</t>
+          <t>Sentence ntr - 140</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Sentence neg - 25</t>
+          <t>Sentence neg - 9</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -463,12 +463,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sentence ntr - 115</t>
+          <t>Sentence ntr - 96</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 48</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -481,12 +481,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Sentence ntr - 92</t>
+          <t>Sentence ntr - 80</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Sentence neg - 127</t>
+          <t>Sentence neg - 136</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -499,12 +499,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sentence ntr - 72</t>
+          <t>Sentence ntr - 87</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sentence neg - 6</t>
+          <t>Sentence neg - 124</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -517,12 +517,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Sentence ntr - 72</t>
+          <t>Sentence ntr - 87</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Sentence neg - 6</t>
+          <t>Sentence neg - 124</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -553,12 +553,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Sentence ntr - 116</t>
+          <t>Sentence ntr - 100</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -571,12 +571,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Sentence ntr - 101</t>
+          <t>Sentence ntr - 86</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 131</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -594,7 +594,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Sentence neg - 123</t>
+          <t>Sentence neg - 121</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -607,12 +607,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Sentence ntr - 102</t>
+          <t>Sentence ntr - 113</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Sentence neg - 135</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -625,12 +625,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Sentence ntr - 105</t>
+          <t>Sentence ntr - 140</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Sentence neg - 15</t>
+          <t>Sentence neg - 48</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -643,12 +643,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Sentence ntr - 92</t>
+          <t>Sentence ntr - 70</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 2</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -661,12 +661,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Sentence ntr - 92</t>
+          <t>Sentence ntr - 70</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Sentence neg - 134</t>
+          <t>Sentence neg - 2</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -679,12 +679,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Sentence ntr - 72</t>
+          <t>Sentence ntr - 96</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Sentence neg - 133</t>
+          <t>Sentence neg - 136</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -697,12 +697,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Sentence neg - 133</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -715,12 +715,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Sentence ntr - 116</t>
+          <t>Sentence ntr - 87</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -733,12 +733,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Sentence ntr - 113</t>
+          <t>Sentence ntr - 86</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Sentence neg - 6</t>
+          <t>Sentence neg - 35</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -751,7 +751,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Sentence ntr - 112</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -769,12 +769,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 9</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -787,12 +787,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -805,12 +805,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Sentence ntr - 115</t>
+          <t>Sentence ntr - 80</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Sentence neg - 127</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -823,12 +823,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Sentence ntr - 102</t>
+          <t>Sentence ntr - 140</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Sentence neg - 16</t>
+          <t>Sentence neg - 136</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -841,12 +841,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Sentence ntr - 105</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -859,12 +859,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 70</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Sentence neg - 6</t>
+          <t>Sentence neg - 124</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -877,12 +877,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 80</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Sentence neg - 6</t>
+          <t>Sentence neg - 48</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -895,12 +895,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Sentence ntr - 112</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Sentence neg - 134</t>
+          <t>Sentence neg - 131</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -913,12 +913,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Sentence ntr - 92</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 131</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -931,12 +931,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Sentence ntr - 103</t>
+          <t>Sentence ntr - 100</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -949,12 +949,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Sentence ntr - 72</t>
+          <t>Sentence ntr - 100</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Sentence neg - 123</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -967,12 +967,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Sentence ntr - 72</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Sentence neg - 135</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -985,12 +985,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Sentence ntr - 113</t>
+          <t>Sentence ntr - 86</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Sentence neg - 25</t>
+          <t>Sentence neg - 121</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1003,12 +1003,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Sentence ntr - 118</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Sentence neg - 25</t>
+          <t>Sentence neg - 2</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1021,12 +1021,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Sentence ntr - 101</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Sentence neg - 15</t>
+          <t>Sentence neg - 35</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1039,12 +1039,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Sentence ntr - 116</t>
+          <t>Sentence ntr - 100</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 2</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1057,12 +1057,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Sentence ntr - 113</t>
+          <t>Sentence ntr - 140</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Sentence neg - 133</t>
+          <t>Sentence neg - 121</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1075,12 +1075,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Sentence ntr - 101</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Sentence neg - 6</t>
+          <t>Sentence neg - 124</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1093,12 +1093,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Sentence ntr - 102</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Sentence neg - 6</t>
+          <t>Sentence neg - 131</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1111,12 +1111,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Sentence ntr - 118</t>
+          <t>Sentence ntr - 96</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Sentence neg - 135</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1129,12 +1129,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Sentence ntr - 72</t>
+          <t>Sentence ntr - 96</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1147,12 +1147,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 70</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Sentence neg - 16</t>
+          <t>Sentence neg - 48</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1165,12 +1165,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 113</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Sentence neg - 123</t>
+          <t>Sentence neg - 35</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1183,12 +1183,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Sentence ntr - 112</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Sentence neg - 123</t>
+          <t>Sentence neg - 9</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1201,12 +1201,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Sentence ntr - 105</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Sentence neg - 127</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1219,12 +1219,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Sentence ntr - 105</t>
+          <t>Sentence ntr - 80</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Sentence neg - 15</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1237,12 +1237,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Sentence ntr - 115</t>
+          <t>Sentence ntr - 87</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Sentence neg - 134</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1255,12 +1255,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Sentence ntr - 113</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Sentence neg - 127</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1273,12 +1273,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Sentence ntr - 72</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Sentence neg - 16</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1291,12 +1291,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Sentence ntr - 105</t>
+          <t>Sentence ntr - 100</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 121</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1309,12 +1309,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Sentence ntr - 105</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 121</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1327,12 +1327,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Sentence ntr - 101</t>
+          <t>Sentence ntr - 80</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Sentence neg - 134</t>
+          <t>Sentence neg - 136</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1345,12 +1345,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 80</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Sentence neg - 134</t>
+          <t>Sentence neg - 136</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1363,7 +1363,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Sentence ntr - 116</t>
+          <t>Sentence ntr - 140</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1381,12 +1381,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Sentence ntr - 103</t>
+          <t>Sentence ntr - 70</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Sentence neg - 25</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1399,12 +1399,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Sentence ntr - 103</t>
+          <t>Sentence ntr - 86</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Sentence neg - 135</t>
+          <t>Sentence neg - 48</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1417,12 +1417,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Sentence neg - 135</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1435,12 +1435,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Sentence ntr - 92</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Sentence neg - 139</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1453,12 +1453,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Sentence ntr - 118</t>
+          <t>Sentence ntr - 113</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Sentence neg - 123</t>
+          <t>Sentence neg - 131</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1471,12 +1471,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Sentence ntr - 112</t>
+          <t>Sentence ntr - 140</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Sentence neg - 123</t>
+          <t>Sentence neg - 35</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1489,12 +1489,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Sentence ntr - 116</t>
+          <t>Sentence ntr - 96</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Sentence neg - 6</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1507,12 +1507,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Sentence ntr - 102</t>
+          <t>Sentence ntr - 70</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Sentence neg - 133</t>
+          <t>Sentence neg - 124</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1525,12 +1525,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Sentence ntr - 72</t>
+          <t>Sentence ntr - 87</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Sentence neg - 133</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1548,7 +1548,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Sentence neg - 127</t>
+          <t>Sentence neg - 2</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1561,12 +1561,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Sentence ntr - 101</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Sentence neg - 16</t>
+          <t>Sentence neg - 2</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1579,12 +1579,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Sentence ntr - 105</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Sentence neg - 139</t>
+          <t>Sentence neg - 136</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1597,12 +1597,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Sentence ntr - 105</t>
+          <t>Sentence ntr - 113</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Sentence neg - 139</t>
+          <t>Sentence neg - 131</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1615,12 +1615,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Sentence neg - 135</t>
+          <t>Sentence neg - 121</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1633,12 +1633,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Sentence neg - 15</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -1651,12 +1651,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 86</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -1669,12 +1669,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Sentence ntr - 92</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Sentence neg - 134</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -1687,12 +1687,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 96</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Sentence neg - 16</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -1705,12 +1705,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Sentence ntr - 118</t>
+          <t>Sentence ntr - 140</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 35</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -1723,12 +1723,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Sentence ntr - 102</t>
+          <t>Sentence ntr - 100</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Sentence neg - 25</t>
+          <t>Sentence neg - 131</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -1741,12 +1741,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Sentence ntr - 102</t>
+          <t>Sentence ntr - 100</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Sentence neg - 25</t>
+          <t>Sentence neg - 124</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -1759,12 +1759,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Sentence ntr - 113</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Sentence neg - 6</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -1777,12 +1777,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Sentence ntr - 72</t>
+          <t>Sentence ntr - 70</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Sentence neg - 133</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -1795,12 +1795,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Sentence ntr - 112</t>
+          <t>Sentence ntr - 86</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -1813,12 +1813,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Sentence neg - 134</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -1831,12 +1831,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Sentence ntr - 103</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1849,12 +1849,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Sentence ntr - 103</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -1872,7 +1872,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Sentence neg - 15</t>
+          <t>Sentence neg - 121</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -1885,12 +1885,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Sentence ntr - 116</t>
+          <t>Sentence ntr - 87</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Sentence neg - 135</t>
+          <t>Sentence neg - 9</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -1903,12 +1903,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Sentence ntr - 116</t>
+          <t>Sentence ntr - 70</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Sentence neg - 25</t>
+          <t>Sentence neg - 2</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -1926,7 +1926,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Sentence neg - 127</t>
+          <t>Sentence neg - 124</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -1939,12 +1939,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Sentence ntr - 92</t>
+          <t>Sentence ntr - 140</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Sentence neg - 16</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -1957,12 +1957,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Sentence ntr - 113</t>
+          <t>Sentence ntr - 140</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Sentence neg - 6</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -1975,12 +1975,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Sentence ntr - 102</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Sentence neg - 123</t>
+          <t>Sentence neg - 9</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -1993,12 +1993,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Sentence ntr - 102</t>
+          <t>Sentence ntr - 113</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Sentence neg - 134</t>
+          <t>Sentence neg - 9</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -2011,12 +2011,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 113</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Sentence neg - 135</t>
+          <t>Sentence neg - 136</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -2029,12 +2029,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Sentence ntr - 105</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Sentence neg - 135</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -2047,12 +2047,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Sentence ntr - 103</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Sentence neg - 15</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -2065,12 +2065,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Sentence ntr - 112</t>
+          <t>Sentence ntr - 80</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -2083,12 +2083,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Sentence ntr - 112</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 121</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -2101,12 +2101,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Sentence ntr - 72</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Sentence neg - 139</t>
+          <t>Sentence neg - 131</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -2119,12 +2119,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Sentence ntr - 105</t>
+          <t>Sentence ntr - 86</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -2137,12 +2137,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Sentence ntr - 116</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Sentence neg - 6</t>
+          <t>Sentence neg - 2</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -2155,12 +2155,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Sentence ntr - 101</t>
+          <t>Sentence ntr - 80</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 9</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -2173,12 +2173,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Sentence ntr - 101</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Sentence neg - 123</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -2191,12 +2191,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Sentence ntr - 102</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Sentence neg - 16</t>
+          <t>Sentence neg - 35</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -2209,12 +2209,12 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Sentence ntr - 115</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Sentence neg - 16</t>
+          <t>Sentence neg - 48</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -2227,12 +2227,12 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Sentence ntr - 92</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -2245,12 +2245,12 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Sentence ntr - 72</t>
+          <t>Sentence ntr - 116</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Sentence neg - 25</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -2263,12 +2263,12 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Sentence neg - 134</t>
+          <t>Sentence neg - 124</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -2281,12 +2281,12 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Sentence ntr - 103</t>
+          <t>Sentence ntr - 96</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Sentence neg - 127</t>
+          <t>Sentence neg - 121</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -2299,12 +2299,12 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Sentence ntr - 103</t>
+          <t>Sentence ntr - 100</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Sentence neg - 127</t>
+          <t>Sentence neg - 121</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -2317,12 +2317,12 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Sentence ntr - 118</t>
+          <t>Sentence ntr - 113</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Sentence neg - 139</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -2335,12 +2335,12 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 100</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Sentence neg - 134</t>
+          <t>Sentence neg - 131</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -2353,12 +2353,12 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Sentence ntr - 72</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Sentence neg - 133</t>
+          <t>Sentence neg - 2</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -2371,12 +2371,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Sentence ntr - 113</t>
+          <t>Sentence ntr - 70</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Sentence neg - 135</t>
+          <t>Sentence neg - 9</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -2389,12 +2389,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Sentence ntr - 113</t>
+          <t>Sentence ntr - 80</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Sentence neg - 135</t>
+          <t>Sentence neg - 9</t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -2407,12 +2407,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Sentence ntr - 118</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Sentence neg - 139</t>
+          <t>Sentence neg - 48</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -2425,12 +2425,12 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Sentence ntr - 105</t>
+          <t>Sentence ntr - 87</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 136</t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -2443,12 +2443,12 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Sentence ntr - 105</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Sentence neg - 25</t>
+          <t>Sentence neg - 121</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -2461,12 +2461,12 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Sentence ntr - 92</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Sentence neg - 25</t>
+          <t>Sentence neg - 35</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -2479,12 +2479,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Sentence ntr - 112</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C118" t="n">
@@ -2497,7 +2497,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Sentence ntr - 116</t>
+          <t>Sentence ntr - 86</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -2515,12 +2515,12 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 86</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Sentence neg - 127</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -2533,12 +2533,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Sentence ntr - 101</t>
+          <t>Sentence ntr - 140</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -2551,12 +2551,12 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Sentence ntr - 102</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Sentence neg - 123</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -2569,12 +2569,12 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Sentence ntr - 115</t>
+          <t>Sentence ntr - 140</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2587,12 +2587,12 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Sentence neg - 127</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -2605,12 +2605,12 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Sentence ntr - 100</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Sentence neg - 127</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C125" t="n">
@@ -2623,12 +2623,12 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Sentence ntr - 92</t>
+          <t>Sentence ntr - 86</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Sentence neg - 25</t>
+          <t>Sentence neg - 124</t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -2641,12 +2641,12 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Sentence ntr - 92</t>
+          <t>Sentence ntr - 87</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 131</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -2659,12 +2659,12 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Sentence ntr - 101</t>
+          <t>Sentence ntr - 100</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Sentence neg - 139</t>
+          <t>Sentence neg - 25</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -2677,12 +2677,12 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Sentence ntr - 116</t>
+          <t>Sentence ntr - 70</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Sentence neg - 139</t>
+          <t>Sentence neg - 2</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -2695,12 +2695,12 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Sentence ntr - 113</t>
+          <t>Sentence ntr - 96</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Sentence neg - 15</t>
+          <t>Sentence neg - 35</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -2713,12 +2713,12 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Sentence ntr - 72</t>
+          <t>Sentence ntr - 113</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Sentence neg - 16</t>
+          <t>Sentence neg - 35</t>
         </is>
       </c>
       <c r="C131" t="n">
@@ -2731,12 +2731,12 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Sentence ntr - 118</t>
+          <t>Sentence ntr - 113</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Sentence neg - 6</t>
+          <t>Sentence neg - 136</t>
         </is>
       </c>
       <c r="C132" t="n">
@@ -2749,12 +2749,12 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Sentence ntr - 112</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Sentence neg - 133</t>
+          <t>Sentence neg - 121</t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -2767,12 +2767,12 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Sentence ntr - 103</t>
+          <t>Sentence ntr - 115</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Sentence neg - 25</t>
+          <t>Sentence neg - 15</t>
         </is>
       </c>
       <c r="C134" t="n">
@@ -2785,12 +2785,12 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Sentence ntr - 101</t>
+          <t>Sentence ntr - 96</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Sentence neg - 125</t>
+          <t>Sentence neg - 35</t>
         </is>
       </c>
       <c r="C135" t="n">
@@ -2803,12 +2803,12 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Sentence ntr - 102</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Sentence neg - 139</t>
+          <t>Sentence neg - 121</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -2821,12 +2821,12 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Sentence ntr - 102</t>
+          <t>Sentence ntr - 117</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Sentence neg - 133</t>
+          <t>Sentence neg - 121</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -2839,12 +2839,12 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Sentence ntr - 92</t>
+          <t>Sentence ntr - 70</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Sentence neg - 15</t>
+          <t>Sentence neg - 131</t>
         </is>
       </c>
       <c r="C138" t="n">
@@ -2857,12 +2857,12 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Sentence ntr - 97</t>
+          <t>Sentence ntr - 80</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Sentence neg - 15</t>
+          <t>Sentence neg - 136</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -2875,12 +2875,12 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Sentence ntr - 116</t>
+          <t>Sentence ntr - 80</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Sentence neg - 124</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -2893,12 +2893,12 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Sentence ntr - 113</t>
+          <t>Sentence ntr - 86</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Sentence neg - 6</t>
+          <t>Sentence neg - 138</t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -2911,12 +2911,12 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Sentence ntr - 113</t>
+          <t>Sentence ntr - 103</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 18</t>
         </is>
       </c>
       <c r="C142" t="n">
@@ -2929,12 +2929,12 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Sentence ntr - 115</t>
+          <t>Sentence ntr - 99</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Sentence neg - 130</t>
+          <t>Sentence neg - 6</t>
         </is>
       </c>
       <c r="C143" t="n">
@@ -2947,12 +2947,12 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Sentence ntr - 105</t>
+          <t>Sentence ntr - 87</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Sentence neg - 16</t>
+          <t>Sentence neg - 124</t>
         </is>
       </c>
       <c r="C144" t="n">
@@ -2965,12 +2965,12 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Sentence ntr - 118</t>
+          <t>Sentence ntr - 100</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Sentence neg - 134</t>
+          <t>Sentence neg - 9</t>
         </is>
       </c>
       <c r="C145" t="n">

</xml_diff>